<commit_message>
changes and allure correction
</commit_message>
<xml_diff>
--- a/demo/src/main/resources/TestCases.xlsx
+++ b/demo/src/main/resources/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82CB0B5-742D-49BD-AD1D-377A929284C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6968FFC6-77E1-4AE4-A1FA-648AEF9A31A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3BD17C19-388F-454B-B009-4EDE4120BD8F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -85,42 +85,6 @@
   </si>
   <si>
     <t>url</t>
-  </si>
-  <si>
-    <t>Test 2</t>
-  </si>
-  <si>
-    <t>Administrator@test.com</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>Test 3</t>
-  </si>
-  <si>
-    <t>//*[@id="MP_link"]</t>
-  </si>
-  <si>
-    <t>//*[@id="menu_time_viewEmployeeTimesheet"]</t>
-  </si>
-  <si>
-    <t>Test 4</t>
-  </si>
-  <si>
-    <t>//*[@id="employee"]</t>
-  </si>
-  <si>
-    <t>//*[@id="btnView"]</t>
-  </si>
-  <si>
-    <t>Charlie Carter</t>
-  </si>
-  <si>
-    <t>Test 5</t>
-  </si>
-  <si>
-    <t>//*[@id="welcome-menu"]/ul/li[3]/a</t>
   </si>
 </sst>
 </file>
@@ -532,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C20C0D85-425A-4DE0-A9C0-9AF6DDCF0671}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,276 +609,33 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>16</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="C18" s="2"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>15</v>
-      </c>
+      <c r="E20" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
@@ -931,10 +652,7 @@
       <c r="E24" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1" xr:uid="{DF14093A-AA74-4205-B65C-1A216B6C59BD}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>